<commit_message>
Carga Proyecto Taltal y correcion errores de carga
</commit_message>
<xml_diff>
--- a/uploads/CategoriaNuevo/CategoriaNueva Taltal.xlsx
+++ b/uploads/CategoriaNuevo/CategoriaNueva Taltal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enami-my.sharepoint.com/personal/pjdiaz_enami_cl/Documents/Escritorio/Proyecto37/Proyecto16/Proyecto11/proyecto2/uploads/CategoriaNuevo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="201" documentId="11_AD4D2F04E46CFB4ACB3E20C07D90DEBA683EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DC273F0-709E-4389-85C5-75E1800F89A5}"/>
+  <xr:revisionPtr revIDLastSave="253" documentId="11_AD4D2F04E46CFB4ACB3E20C07D90DEBA683EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CE942D3-ED87-469F-A397-F9D9F64442AE}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
   <si>
     <t>id</t>
   </si>
@@ -157,6 +157,192 @@
   </si>
   <si>
     <t>Comisionamiento</t>
+  </si>
+  <si>
+    <t>Costos Adicionales</t>
+  </si>
+  <si>
+    <t>Costos del dueño</t>
+  </si>
+  <si>
+    <t>Gastos Generales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUADRO  ELEMENTOS PRINCIPALES ILUMINACION EXTERIOR Y TDA SECTOR </t>
+  </si>
+  <si>
+    <t>POSTES DE HORMIGON ARMADO 8.7 M</t>
+  </si>
+  <si>
+    <t>CABLE DE ALUMINIO PREEMSAMBLADO 3x35 mm2 + 50 mm2</t>
+  </si>
+  <si>
+    <t>TIRANTE COMPLETO BAJA TENSION</t>
+  </si>
+  <si>
+    <t>LUMINARIA BLESTED LED 200W (Certificada)</t>
+  </si>
+  <si>
+    <t>GANCHO NORMA NACIONAL Brazo acero Galvanizado para Lum L-150 1 1/2" X3Mt</t>
+  </si>
+  <si>
+    <t>PORTA FUSIBLE AEREO CON FUSIBLE 1 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOPORTE DE REMATE </t>
+  </si>
+  <si>
+    <t>SOPORTE DE PASO</t>
+  </si>
+  <si>
+    <t>CONJUNTO FERRETERIA ACERO GALVANIZADA</t>
+  </si>
+  <si>
+    <t>TABLERO METALICO 600X500X230 mm C/PUERTA INTERIOR</t>
+  </si>
+  <si>
+    <t>INTERRUPTOR TERMOMAGNETICO 3P 40A   C 10KA</t>
+  </si>
+  <si>
+    <t>INT. TERMOMAGNETICO CURVA C 230/400VAC Icu=10kA</t>
+  </si>
+  <si>
+    <t>INTERRUPTOR TERMOMAGNETICO 3P 10A   C 10KA</t>
+  </si>
+  <si>
+    <t>INTERRUPTOR TERMOMAGNETICO 3P 32A   C 10KA</t>
+  </si>
+  <si>
+    <t>INTERRUPTOR TERMOMAGNETICO 1P 2A   C 10KA</t>
+  </si>
+  <si>
+    <t>INTERRUPTOR DIFERENCIAL 4P 16A   AC 10KA</t>
+  </si>
+  <si>
+    <t>CONTACTOR SCHNEIDER 380 V - BOBINA 220 V</t>
+  </si>
+  <si>
+    <t>RELOJ HORARIO CON RESERVA UNO-QRD 220VAC 16A 50/60HZ</t>
+  </si>
+  <si>
+    <t>LAMPARA PILOTO ROJA 230AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REPARTIDOR TETRAPOLAR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECTOR 3 POSICIONES 1NA+1NC </t>
+  </si>
+  <si>
+    <t>BARRA TOMA A TIERRA</t>
+  </si>
+  <si>
+    <t>CANALETA RANURADA 40X40MM</t>
+  </si>
+  <si>
+    <t>BORNES DE CONEXION 4 mm2 VIKING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUSIBLE Y PORTAFUSIBLE MONOPOLAR 10*38 </t>
+  </si>
+  <si>
+    <t>Tubo Pvc Schedule 40 3"X6Mt (Linea Subterranea)</t>
+  </si>
+  <si>
+    <t>Elementos electricos e Instrumentos</t>
+  </si>
+  <si>
+    <t>CUADRO DE ELEMENTOS PRINCIPALES TDFyC PISCINA ACUMULADORA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERRUPTOR TERMOMAGNETICO </t>
+  </si>
+  <si>
+    <t>CABLE SUPERFLEX/MULTIFLEX 4X4 AWG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABLE SUPERFLEX/MULTIFLEX 4X6 AWG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT. TERMOMAGNETICO CURVA C, 10 KA </t>
+  </si>
+  <si>
+    <t>DIFERENCIAL  (2x16A)</t>
+  </si>
+  <si>
+    <t>RELE TERMICO MOTOR EasyPact TVS - 12...18A</t>
+  </si>
+  <si>
+    <t>CONTACTOR 25A 380V 1Na+1Nc 220Vca</t>
+  </si>
+  <si>
+    <t>RELE UNIV 11P 230VAC 10A 3NA/3NC MAS SOCALO O BASE</t>
+  </si>
+  <si>
+    <t>GABINETE METALICO 2 PUERTAS 600X500X200 IP65</t>
+  </si>
+  <si>
+    <t>PULSADOR PARADA EMERGENCIA 22 mm 1Nc Girar para Desenclavar</t>
+  </si>
+  <si>
+    <t>SELECTOR 3 POSICIONES CON RETENCION 2NA+2NC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECTOR CONMUTADOR BOMBAS ALTERNADAS, 0-B1-B2-ALT, 48X48MM </t>
+  </si>
+  <si>
+    <t>RM35LM33MW ZELIO CONTROL NIVEL LIQUIDOS POR SONDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SONDA DE NIVEL LIQUIDO LA9RM201</t>
+  </si>
+  <si>
+    <t>LAMPARA PILOTO LED VERDE</t>
+  </si>
+  <si>
+    <t>LAMPARA PILOTO LED ROJA</t>
+  </si>
+  <si>
+    <t>BALIZA LUZ FIJA/INTERMITENTE ROJA 24-230VCA</t>
+  </si>
+  <si>
+    <t>FUSIBLE Y PORTAFUSIBLE 2A</t>
+  </si>
+  <si>
+    <t>ELEMENTOS MALLA A TIERRA (INCLUIDAS LAS DOS MALLAS)</t>
+  </si>
+  <si>
+    <t>CONDUCTOR CU DESNUDO 33.6 mm2</t>
+  </si>
+  <si>
+    <t>CONDUCTOR SPFLEX 4AWG</t>
+  </si>
+  <si>
+    <t>DUCTO c.a.g1" 3MT</t>
+  </si>
+  <si>
+    <t>CAPSULA PARA SOLDAR</t>
+  </si>
+  <si>
+    <t>CABLE DESNUDO 2AWG</t>
+  </si>
+  <si>
+    <t>SAL ERICO GEL 11KG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barra Toma Tierra 5/8' X1mt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRENSA TOMATIERRA 600 AMP </t>
+  </si>
+  <si>
+    <t>TUBO CONCRETO 200mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAPA CONCRETO </t>
+  </si>
+  <si>
+    <t>MOLDE DE GRAFITO TIPO T 2 AWG</t>
   </si>
 </sst>
 </file>
@@ -208,7 +394,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,8 +419,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -288,11 +486,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -323,6 +534,24 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,15 +833,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35:G39"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="45.453125" customWidth="1"/>
+    <col min="2" max="2" width="60.08984375" customWidth="1"/>
     <col min="3" max="4" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1502,6 +1731,1558 @@
         <v>0</v>
       </c>
     </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>46038</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>46038</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="9">
+        <v>46039</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="E41" s="9">
+        <v>46039</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>46040</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="E42">
+        <v>46040</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="15">
+        <v>46041</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="15">
+        <v>3</v>
+      </c>
+      <c r="E43" s="15">
+        <v>46041</v>
+      </c>
+      <c r="F43" s="15">
+        <v>1</v>
+      </c>
+      <c r="G43" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="17">
+        <v>46042</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="17">
+        <v>3</v>
+      </c>
+      <c r="D44" s="17">
+        <v>46041</v>
+      </c>
+      <c r="E44" s="17">
+        <v>46042</v>
+      </c>
+      <c r="F44" s="17">
+        <v>2</v>
+      </c>
+      <c r="G44" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="9">
+        <v>46043</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>46042</v>
+      </c>
+      <c r="E45" s="9">
+        <v>46043</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>46044</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>46042</v>
+      </c>
+      <c r="E46">
+        <v>46044</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="9">
+        <v>46045</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>46042</v>
+      </c>
+      <c r="E47" s="9">
+        <v>46045</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>46046</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>46042</v>
+      </c>
+      <c r="E48">
+        <v>46046</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="9">
+        <v>46047</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>46042</v>
+      </c>
+      <c r="E49" s="9">
+        <v>46047</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>46048</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>46042</v>
+      </c>
+      <c r="E50">
+        <v>46048</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="9">
+        <v>46049</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <v>46042</v>
+      </c>
+      <c r="E51" s="9">
+        <v>46049</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>46050</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <v>46042</v>
+      </c>
+      <c r="E52">
+        <v>46050</v>
+      </c>
+      <c r="F52">
+        <v>3</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="9">
+        <v>46051</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>46042</v>
+      </c>
+      <c r="E53" s="9">
+        <v>46051</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>46052</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <v>46042</v>
+      </c>
+      <c r="E54">
+        <v>46052</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="9">
+        <v>46053</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>46042</v>
+      </c>
+      <c r="E55" s="9">
+        <v>46053</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>46054</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56">
+        <v>46042</v>
+      </c>
+      <c r="E56">
+        <v>46054</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="9">
+        <v>46055</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57">
+        <v>46042</v>
+      </c>
+      <c r="E57" s="9">
+        <v>46055</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>46056</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58">
+        <v>46042</v>
+      </c>
+      <c r="E58">
+        <v>46056</v>
+      </c>
+      <c r="F58">
+        <v>3</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="9">
+        <v>46057</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59">
+        <v>46042</v>
+      </c>
+      <c r="E59" s="9">
+        <v>46057</v>
+      </c>
+      <c r="F59">
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>46058</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60">
+        <v>46042</v>
+      </c>
+      <c r="E60">
+        <v>46058</v>
+      </c>
+      <c r="F60">
+        <v>3</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="9">
+        <v>46059</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <v>46042</v>
+      </c>
+      <c r="E61" s="9">
+        <v>46059</v>
+      </c>
+      <c r="F61">
+        <v>3</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>46060</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>46042</v>
+      </c>
+      <c r="E62">
+        <v>46060</v>
+      </c>
+      <c r="F62">
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="9">
+        <v>46061</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <v>46042</v>
+      </c>
+      <c r="E63" s="9">
+        <v>46061</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>46062</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
+      </c>
+      <c r="D64">
+        <v>46042</v>
+      </c>
+      <c r="E64">
+        <v>46062</v>
+      </c>
+      <c r="F64">
+        <v>3</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="9">
+        <v>46063</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65">
+        <v>46042</v>
+      </c>
+      <c r="E65" s="9">
+        <v>46063</v>
+      </c>
+      <c r="F65">
+        <v>3</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>46064</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66">
+        <v>46042</v>
+      </c>
+      <c r="E66">
+        <v>46064</v>
+      </c>
+      <c r="F66">
+        <v>3</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" s="9">
+        <v>46065</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67">
+        <v>46042</v>
+      </c>
+      <c r="E67" s="9">
+        <v>46065</v>
+      </c>
+      <c r="F67">
+        <v>3</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>46066</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68">
+        <v>46042</v>
+      </c>
+      <c r="E68">
+        <v>46066</v>
+      </c>
+      <c r="F68">
+        <v>3</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="9">
+        <v>46067</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69">
+        <v>46042</v>
+      </c>
+      <c r="E69" s="9">
+        <v>46067</v>
+      </c>
+      <c r="F69">
+        <v>3</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>46068</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70">
+        <v>46042</v>
+      </c>
+      <c r="E70">
+        <v>46068</v>
+      </c>
+      <c r="F70">
+        <v>3</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="17">
+        <v>46069</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71" s="17">
+        <v>3</v>
+      </c>
+      <c r="D71" s="17">
+        <v>46041</v>
+      </c>
+      <c r="E71" s="17">
+        <v>46069</v>
+      </c>
+      <c r="F71" s="17">
+        <v>2</v>
+      </c>
+      <c r="G71" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="18">
+        <v>46070</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72" s="18">
+        <v>3</v>
+      </c>
+      <c r="D72" s="18">
+        <v>46069</v>
+      </c>
+      <c r="E72" s="18">
+        <v>46070</v>
+      </c>
+      <c r="F72" s="18">
+        <v>3</v>
+      </c>
+      <c r="G72" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" s="9">
+        <v>46071</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73">
+        <v>46069</v>
+      </c>
+      <c r="E73" s="9">
+        <v>46071</v>
+      </c>
+      <c r="F73">
+        <v>3</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>46072</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74">
+        <v>46069</v>
+      </c>
+      <c r="E74">
+        <v>46072</v>
+      </c>
+      <c r="F74">
+        <v>3</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" s="9">
+        <v>46073</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75">
+        <v>46069</v>
+      </c>
+      <c r="E75" s="9">
+        <v>46073</v>
+      </c>
+      <c r="F75">
+        <v>3</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>46074</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76">
+        <v>46069</v>
+      </c>
+      <c r="E76">
+        <v>46074</v>
+      </c>
+      <c r="F76">
+        <v>3</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" s="9">
+        <v>46075</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77">
+        <v>46069</v>
+      </c>
+      <c r="E77" s="9">
+        <v>46075</v>
+      </c>
+      <c r="F77">
+        <v>3</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>46076</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78">
+        <v>46069</v>
+      </c>
+      <c r="E78">
+        <v>46076</v>
+      </c>
+      <c r="F78">
+        <v>3</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A79" s="9">
+        <v>46077</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79">
+        <v>46069</v>
+      </c>
+      <c r="E79" s="9">
+        <v>46077</v>
+      </c>
+      <c r="F79">
+        <v>3</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>46078</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="D80">
+        <v>46069</v>
+      </c>
+      <c r="E80">
+        <v>46078</v>
+      </c>
+      <c r="F80">
+        <v>3</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" s="9">
+        <v>46079</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C81">
+        <v>3</v>
+      </c>
+      <c r="D81">
+        <v>46069</v>
+      </c>
+      <c r="E81" s="9">
+        <v>46079</v>
+      </c>
+      <c r="F81">
+        <v>3</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>46080</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C82">
+        <v>3</v>
+      </c>
+      <c r="D82">
+        <v>46069</v>
+      </c>
+      <c r="E82">
+        <v>46080</v>
+      </c>
+      <c r="F82">
+        <v>3</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="9">
+        <v>46081</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C83">
+        <v>3</v>
+      </c>
+      <c r="D83">
+        <v>46069</v>
+      </c>
+      <c r="E83" s="9">
+        <v>46081</v>
+      </c>
+      <c r="F83">
+        <v>3</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>46082</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84">
+        <v>3</v>
+      </c>
+      <c r="D84">
+        <v>46069</v>
+      </c>
+      <c r="E84">
+        <v>46082</v>
+      </c>
+      <c r="F84">
+        <v>3</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A85" s="9">
+        <v>46083</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C85">
+        <v>3</v>
+      </c>
+      <c r="D85">
+        <v>46069</v>
+      </c>
+      <c r="E85" s="9">
+        <v>46083</v>
+      </c>
+      <c r="F85">
+        <v>3</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>46084</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86">
+        <v>46069</v>
+      </c>
+      <c r="E86">
+        <v>46084</v>
+      </c>
+      <c r="F86">
+        <v>3</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="9">
+        <v>46085</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87">
+        <v>46069</v>
+      </c>
+      <c r="E87" s="9">
+        <v>46085</v>
+      </c>
+      <c r="F87">
+        <v>3</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>46086</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88">
+        <v>46069</v>
+      </c>
+      <c r="E88">
+        <v>46086</v>
+      </c>
+      <c r="F88">
+        <v>3</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" s="9">
+        <v>46087</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
+      </c>
+      <c r="D89">
+        <v>46069</v>
+      </c>
+      <c r="E89" s="9">
+        <v>46087</v>
+      </c>
+      <c r="F89">
+        <v>3</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>46088</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C90">
+        <v>3</v>
+      </c>
+      <c r="D90">
+        <v>46069</v>
+      </c>
+      <c r="E90">
+        <v>46088</v>
+      </c>
+      <c r="F90">
+        <v>3</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" s="9">
+        <v>46089</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
+      </c>
+      <c r="D91">
+        <v>46069</v>
+      </c>
+      <c r="E91" s="9">
+        <v>46089</v>
+      </c>
+      <c r="F91">
+        <v>3</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>46090</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C92">
+        <v>3</v>
+      </c>
+      <c r="D92">
+        <v>46069</v>
+      </c>
+      <c r="E92">
+        <v>46090</v>
+      </c>
+      <c r="F92">
+        <v>3</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" s="9">
+        <v>46091</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C93">
+        <v>3</v>
+      </c>
+      <c r="D93">
+        <v>46069</v>
+      </c>
+      <c r="E93" s="9">
+        <v>46091</v>
+      </c>
+      <c r="F93">
+        <v>3</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>46092</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C94">
+        <v>3</v>
+      </c>
+      <c r="D94">
+        <v>46069</v>
+      </c>
+      <c r="E94">
+        <v>46092</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="9">
+        <v>46093</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
+      </c>
+      <c r="D95">
+        <v>46069</v>
+      </c>
+      <c r="E95" s="9">
+        <v>46093</v>
+      </c>
+      <c r="F95">
+        <v>3</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>46094</v>
+      </c>
+      <c r="B96" t="s">
+        <v>94</v>
+      </c>
+      <c r="C96">
+        <v>3</v>
+      </c>
+      <c r="D96">
+        <v>46041</v>
+      </c>
+      <c r="E96">
+        <v>46094</v>
+      </c>
+      <c r="F96">
+        <v>2</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A97" s="9">
+        <v>46095</v>
+      </c>
+      <c r="B97" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C97">
+        <v>3</v>
+      </c>
+      <c r="D97">
+        <v>46094</v>
+      </c>
+      <c r="E97" s="9">
+        <v>46095</v>
+      </c>
+      <c r="F97">
+        <v>3</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>46096</v>
+      </c>
+      <c r="B98" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C98">
+        <v>3</v>
+      </c>
+      <c r="D98">
+        <v>46094</v>
+      </c>
+      <c r="E98">
+        <v>46096</v>
+      </c>
+      <c r="F98">
+        <v>3</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99" s="9">
+        <v>46097</v>
+      </c>
+      <c r="B99" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C99">
+        <v>3</v>
+      </c>
+      <c r="D99">
+        <v>46094</v>
+      </c>
+      <c r="E99" s="9">
+        <v>46097</v>
+      </c>
+      <c r="F99">
+        <v>3</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>46098</v>
+      </c>
+      <c r="B100" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C100">
+        <v>3</v>
+      </c>
+      <c r="D100">
+        <v>46094</v>
+      </c>
+      <c r="E100">
+        <v>46098</v>
+      </c>
+      <c r="F100">
+        <v>3</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A101" s="9">
+        <v>46099</v>
+      </c>
+      <c r="B101" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C101">
+        <v>3</v>
+      </c>
+      <c r="D101">
+        <v>46094</v>
+      </c>
+      <c r="E101" s="9">
+        <v>46099</v>
+      </c>
+      <c r="F101">
+        <v>3</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>46100</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C102">
+        <v>3</v>
+      </c>
+      <c r="D102">
+        <v>46094</v>
+      </c>
+      <c r="E102">
+        <v>46100</v>
+      </c>
+      <c r="F102">
+        <v>3</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A103" s="9">
+        <v>46101</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C103">
+        <v>3</v>
+      </c>
+      <c r="D103">
+        <v>46094</v>
+      </c>
+      <c r="E103" s="9">
+        <v>46101</v>
+      </c>
+      <c r="F103">
+        <v>3</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>46102</v>
+      </c>
+      <c r="B104" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
+      </c>
+      <c r="D104">
+        <v>46094</v>
+      </c>
+      <c r="E104">
+        <v>46102</v>
+      </c>
+      <c r="F104">
+        <v>3</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A105" s="9">
+        <v>46103</v>
+      </c>
+      <c r="B105" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C105">
+        <v>3</v>
+      </c>
+      <c r="D105">
+        <v>46094</v>
+      </c>
+      <c r="E105" s="9">
+        <v>46103</v>
+      </c>
+      <c r="F105">
+        <v>3</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>46104</v>
+      </c>
+      <c r="B106" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C106">
+        <v>3</v>
+      </c>
+      <c r="D106">
+        <v>46094</v>
+      </c>
+      <c r="E106">
+        <v>46104</v>
+      </c>
+      <c r="F106">
+        <v>3</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A107" s="9">
+        <v>46105</v>
+      </c>
+      <c r="B107" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C107">
+        <v>3</v>
+      </c>
+      <c r="D107">
+        <v>46094</v>
+      </c>
+      <c r="E107" s="9">
+        <v>46105</v>
+      </c>
+      <c r="F107">
+        <v>3</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>